<commit_message>
New attributes have been added to the condition elements, such as the language of the data field and several general improvements for the use of conditions
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample03-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample03-from-config-file.xlsx
@@ -622,8 +622,8 @@
   <cols>
     <col min="1" max="1" width="11.8295484270368" customWidth="1"/>
     <col min="2" max="2" width="10.0456025259835" customWidth="1"/>
-    <col min="3" max="3" width="8.91818455287388" customWidth="1"/>
-    <col min="4" max="4" width="7.42655563354492" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="16.8203408377511" customWidth="1"/>
     <col min="6" max="6" width="16.8101109095982" customWidth="1"/>
     <col min="7" max="7" width="11.6947838919503" customWidth="1"/>

</xml_diff>